<commit_message>
HOT-118 - Multi retrieval tested in MyBatis.
</commit_message>
<xml_diff>
--- a/hotrod/docs/identity-keys-research/summary.xlsx
+++ b/hotrod/docs/identity-keys-research/summary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,165 +20,222 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="53">
-  <si>
-    <t xml:space="preserve">Column auto-generated by</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supports Identity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JDBC Retrieves Generated Identity Keys</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sequence Strategy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identity Strategy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Default Strategy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Combined Retrieval</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sequence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identity Always</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identity By Default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pre Insert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Combi ned</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Post Insert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Strategy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multiple Values</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEQs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IDENTs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEFs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEQ post insert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Apache Derby  10.13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Single</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GK, RN, RI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DB2 10.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RN, RI, QS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">values PREVIOUS VALUE FOR gen_seq1, PREVIOUS VALUE FOR gen_seq1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H2 1.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Y*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Y**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">values currval('gen_seq1'), currval('gen_seq2')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HyperSQL 2.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GK, RI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MariaDB 5.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N/A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MySQL 5.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oracle 10g</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RN, RI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select gen_seq1.currval, gen_seq2.currval from dual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oracle 12c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PostgreSQL 9.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multiple</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RN, QR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select currval('gen_seq1'), currval('gen_seq2')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAP ASE 16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SQL Server 2014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Max one value returned</t>
-  </si>
-  <si>
-    <t xml:space="preserve">** Unreliable when combined with triggers.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="72">
+  <si>
+    <t>Column auto-generated by</t>
+  </si>
+  <si>
+    <t>Supports Identity</t>
+  </si>
+  <si>
+    <t>JDBC Retrieves Generated Identity Keys</t>
+  </si>
+  <si>
+    <t>Sequence Strategy</t>
+  </si>
+  <si>
+    <t>Identity Strategy</t>
+  </si>
+  <si>
+    <t>Default Strategy</t>
+  </si>
+  <si>
+    <t>Combined Retrieval</t>
+  </si>
+  <si>
+    <t>Sequence</t>
+  </si>
+  <si>
+    <t>Identity Always</t>
+  </si>
+  <si>
+    <t>Identity By Default</t>
+  </si>
+  <si>
+    <t>Pre Insert</t>
+  </si>
+  <si>
+    <t>Combi ned</t>
+  </si>
+  <si>
+    <t>Post Insert</t>
+  </si>
+  <si>
+    <t>Strategy</t>
+  </si>
+  <si>
+    <t>Multiple Values</t>
+  </si>
+  <si>
+    <t>SEQs</t>
+  </si>
+  <si>
+    <t>IDENTs</t>
+  </si>
+  <si>
+    <t>DEFs</t>
+  </si>
+  <si>
+    <t>SEQ post insert</t>
+  </si>
+  <si>
+    <t>Apache Derby  10.13</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>N?</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>GK, RN, RI</t>
+  </si>
+  <si>
+    <t>DB2 10.5</t>
+  </si>
+  <si>
+    <t>***</t>
+  </si>
+  <si>
+    <t>RN, RI, QS</t>
+  </si>
+  <si>
+    <t>values PREVIOUS VALUE FOR gen_seq1, PREVIOUS VALUE FOR gen_seq1</t>
+  </si>
+  <si>
+    <t>H2 1.3</t>
+  </si>
+  <si>
+    <t>Y*</t>
+  </si>
+  <si>
+    <t>Y**</t>
+  </si>
+  <si>
+    <t>values currval('gen_seq1'), currval('gen_seq2')</t>
+  </si>
+  <si>
+    <t>HyperSQL 2.2</t>
+  </si>
+  <si>
+    <t>GK, RI</t>
+  </si>
+  <si>
+    <t>MariaDB 5.5</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>**</t>
+  </si>
+  <si>
+    <t>MySQL 5.5</t>
+  </si>
+  <si>
+    <t>Oracle 10g</t>
+  </si>
+  <si>
+    <t>RN, RI</t>
+  </si>
+  <si>
+    <t>select gen_seq1.currval, gen_seq2.currval from dual</t>
+  </si>
+  <si>
+    <t>Oracle 12c</t>
+  </si>
+  <si>
+    <t>“</t>
+  </si>
+  <si>
+    <t>PostgreSQL 9.4</t>
+  </si>
+  <si>
+    <t>Multiple</t>
+  </si>
+  <si>
+    <t>RN, QR</t>
+  </si>
+  <si>
+    <t>select currval('gen_seq1'), currval('gen_seq2')</t>
+  </si>
+  <si>
+    <t>SAP ASE 16</t>
+  </si>
+  <si>
+    <t>SQL Server 2014</t>
+  </si>
+  <si>
+    <t>QO</t>
+  </si>
+  <si>
+    <t>SQLite</t>
+  </si>
+  <si>
+    <t>Teradata</t>
+  </si>
+  <si>
+    <t>Y?</t>
+  </si>
+  <si>
+    <t>* Max one value returned</t>
+  </si>
+  <si>
+    <t>** Unreliable when combined with triggers.</t>
+  </si>
+  <si>
+    <t>Grupo 1 - Integrado: [insert + identity + seq + default]</t>
+  </si>
+  <si>
+    <t>RN</t>
+  </si>
+  <si>
+    <t>DB2</t>
+  </si>
+  <si>
+    <t>Oracle</t>
+  </si>
+  <si>
+    <t>PostgreSQL</t>
+  </si>
+  <si>
+    <t>SQL Server</t>
+  </si>
+  <si>
+    <t>Grupo 2 - Semi Integrado [seq] -&gt; [insert + identity] -&gt; [default]</t>
+  </si>
+  <si>
+    <t>SAP ASE</t>
+  </si>
+  <si>
+    <t>MySQL</t>
+  </si>
+  <si>
+    <t>MariaDB</t>
+  </si>
+  <si>
+    <t>GK</t>
+  </si>
+  <si>
+    <t>HyperSQL</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>Apache Derby</t>
+  </si>
+  <si>
+    <t>Grupo 3 - Rudimentario [seq] -&gt; [insert] -&gt; [identity] -&gt; [default]</t>
   </si>
 </sst>
 </file>
@@ -186,7 +243,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -245,8 +302,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFCCFFFF"/>
+        <bgColor rgb="FFE6E6FF"/>
       </patternFill>
     </fill>
     <fill>
@@ -321,7 +378,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -370,10 +427,22 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -388,6 +457,26 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -420,7 +509,7 @@
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFE6E6FF"/>
+      <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
@@ -434,7 +523,7 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFE6E6FF"/>
       <rgbColor rgb="FFCCFF99"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
@@ -467,26 +556,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:W17"/>
+  <dimension ref="B1:W33"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="topRight" activeCell="P1" activeCellId="0" sqref="P1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q20" activeCellId="0" sqref="Q20"/>
+      <selection pane="bottomRight" activeCell="Q36" activeCellId="0" sqref="Q36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.64285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="15" min="10" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="12.0867346938776"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="64.9285714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="15" min="10" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="22" min="18" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="63.4438775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="24" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -616,10 +709,12 @@
       <c r="O4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="P4" s="0"/>
-      <c r="Q4" s="12" t="s">
+      <c r="P4" s="12" t="s">
         <v>24</v>
       </c>
+      <c r="Q4" s="13" t="s">
+        <v>25</v>
+      </c>
       <c r="R4" s="9" t="s">
         <v>20</v>
       </c>
@@ -634,8 +729,8 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="8" t="s">
-        <v>25</v>
+      <c r="B5" s="14" t="s">
+        <v>26</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>20</v>
@@ -670,12 +765,12 @@
       <c r="O5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="P5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q5" s="12" t="s">
+      <c r="P5" s="12" t="s">
         <v>27</v>
       </c>
+      <c r="Q5" s="15" t="s">
+        <v>28</v>
+      </c>
       <c r="R5" s="9" t="s">
         <v>20</v>
       </c>
@@ -688,13 +783,13 @@
       <c r="U5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="W5" s="13" t="s">
-        <v>28</v>
+      <c r="W5" s="16" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
-        <v>29</v>
+      <c r="B6" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>20</v>
@@ -715,7 +810,7 @@
         <v>20</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L6" s="9" t="s">
         <v>20</v>
@@ -723,16 +818,18 @@
       <c r="M6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="N6" s="14" t="s">
-        <v>31</v>
+      <c r="N6" s="17" t="s">
+        <v>32</v>
       </c>
       <c r="O6" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="P6" s="0"/>
-      <c r="Q6" s="12" t="s">
+      <c r="P6" s="12" t="s">
         <v>24</v>
       </c>
+      <c r="Q6" s="13" t="s">
+        <v>25</v>
+      </c>
       <c r="R6" s="11" t="s">
         <v>22</v>
       </c>
@@ -745,13 +842,13 @@
       <c r="U6" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="W6" s="15" t="s">
-        <v>32</v>
+      <c r="W6" s="18" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="s">
-        <v>33</v>
+      <c r="B7" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>20</v>
@@ -786,9 +883,11 @@
       <c r="O7" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="P7" s="0"/>
-      <c r="Q7" s="12" t="s">
-        <v>34</v>
+      <c r="P7" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q7" s="13" t="s">
+        <v>35</v>
       </c>
       <c r="R7" s="9" t="s">
         <v>20</v>
@@ -804,8 +903,8 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="s">
-        <v>35</v>
+      <c r="B8" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>22</v>
@@ -822,14 +921,14 @@
       <c r="H8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="K8" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="L8" s="16" t="s">
-        <v>36</v>
+      <c r="J8" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="L8" s="19" t="s">
+        <v>37</v>
       </c>
       <c r="M8" s="9" t="s">
         <v>20</v>
@@ -840,17 +939,17 @@
       <c r="O8" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="P8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q8" s="12" t="s">
-        <v>24</v>
+      <c r="P8" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q8" s="13" t="s">
+        <v>25</v>
       </c>
       <c r="R8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="S8" s="16" t="s">
-        <v>36</v>
+      <c r="S8" s="19" t="s">
+        <v>37</v>
       </c>
       <c r="T8" s="9" t="s">
         <v>20</v>
@@ -860,8 +959,8 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0" t="s">
-        <v>38</v>
+      <c r="B9" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>22</v>
@@ -878,14 +977,14 @@
       <c r="H9" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="J9" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="K9" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="L9" s="16" t="s">
-        <v>36</v>
+      <c r="J9" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="K9" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="L9" s="19" t="s">
+        <v>37</v>
       </c>
       <c r="M9" s="9" t="s">
         <v>20</v>
@@ -896,17 +995,17 @@
       <c r="O9" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="P9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q9" s="12" t="s">
-        <v>24</v>
+      <c r="P9" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q9" s="13" t="s">
+        <v>25</v>
       </c>
       <c r="R9" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="S9" s="16" t="s">
-        <v>36</v>
+      <c r="S9" s="19" t="s">
+        <v>37</v>
       </c>
       <c r="T9" s="9" t="s">
         <v>20</v>
@@ -916,8 +1015,8 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="8" t="s">
-        <v>39</v>
+      <c r="B10" s="14" t="s">
+        <v>40</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>20</v>
@@ -928,8 +1027,8 @@
       <c r="E10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="16" t="s">
-        <v>36</v>
+      <c r="F10" s="19" t="s">
+        <v>37</v>
       </c>
       <c r="H10" s="11" t="s">
         <v>22</v>
@@ -943,20 +1042,20 @@
       <c r="L10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="M10" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="N10" s="16" t="s">
-        <v>36</v>
+      <c r="M10" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="N10" s="19" t="s">
+        <v>37</v>
       </c>
       <c r="O10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="P10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q10" s="12" t="s">
-        <v>40</v>
+      <c r="P10" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q10" s="15" t="s">
+        <v>41</v>
       </c>
       <c r="R10" s="9" t="s">
         <v>20</v>
@@ -964,19 +1063,19 @@
       <c r="S10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="T10" s="16" t="s">
-        <v>36</v>
+      <c r="T10" s="19" t="s">
+        <v>37</v>
       </c>
       <c r="U10" s="9" t="s">
         <v>20</v>
       </c>
       <c r="W10" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="8" t="s">
-        <v>42</v>
+      <c r="B11" s="14" t="s">
+        <v>43</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>20</v>
@@ -1011,11 +1110,11 @@
       <c r="O11" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="P11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q11" s="12" t="s">
-        <v>40</v>
+      <c r="P11" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q11" s="15" t="s">
+        <v>41</v>
       </c>
       <c r="R11" s="9" t="s">
         <v>20</v>
@@ -1030,12 +1129,12 @@
         <v>20</v>
       </c>
       <c r="W11" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="8" t="s">
-        <v>44</v>
+      <c r="B12" s="14" t="s">
+        <v>45</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>20</v>
@@ -1047,7 +1146,7 @@
         <v>20</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H12" s="11" t="s">
         <v>22</v>
@@ -1064,17 +1163,17 @@
       <c r="M12" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="N12" s="14" t="s">
-        <v>31</v>
+      <c r="N12" s="17" t="s">
+        <v>32</v>
       </c>
       <c r="O12" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="P12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q12" s="12" t="s">
-        <v>46</v>
+      <c r="P12" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q12" s="13" t="s">
+        <v>47</v>
       </c>
       <c r="R12" s="9" t="s">
         <v>20</v>
@@ -1089,12 +1188,12 @@
         <v>20</v>
       </c>
       <c r="W12" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>22</v>
@@ -1111,14 +1210,14 @@
       <c r="H13" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="K13" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="L13" s="16" t="s">
-        <v>36</v>
+      <c r="J13" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="K13" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="L13" s="19" t="s">
+        <v>37</v>
       </c>
       <c r="M13" s="9" t="s">
         <v>20</v>
@@ -1129,17 +1228,17 @@
       <c r="O13" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="P13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q13" s="12" t="s">
-        <v>24</v>
+      <c r="P13" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q13" s="13" t="s">
+        <v>25</v>
       </c>
       <c r="R13" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="S13" s="16" t="s">
-        <v>36</v>
+      <c r="S13" s="19" t="s">
+        <v>37</v>
       </c>
       <c r="T13" s="9" t="s">
         <v>20</v>
@@ -1150,7 +1249,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>20</v>
@@ -1185,11 +1284,11 @@
       <c r="O14" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="P14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q14" s="12" t="s">
-        <v>50</v>
+      <c r="P14" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q14" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="R14" s="9" t="s">
         <v>20</v>
@@ -1204,13 +1303,192 @@
         <v>20</v>
       </c>
     </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="20"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="22"/>
+      <c r="Q15" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="R15" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="S15" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="T15" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="U15" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="V15" s="21"/>
+    </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J16" s="0" t="s">
+      <c r="B16" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="20"/>
+      <c r="E16" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="20"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="20"/>
+      <c r="P16" s="22"/>
+      <c r="Q16" s="20"/>
+      <c r="R16" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="S16" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="T16" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="U16" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="V16" s="21"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J18" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J19" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q19" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q20" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="R20" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q21" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="R21" s="24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q22" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="R22" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q23" s="12" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J17" s="0" t="s">
+      <c r="R23" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q24" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q25" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="R25" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q26" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="R26" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q27" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="R27" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q28" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="R28" s="18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q29" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="R29" s="24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q30" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="R30" s="18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R31" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q32" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R33" s="0" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>

<commit_message>
HOT-118 - Studying default, identity, sequences.
</commit_message>
<xml_diff>
--- a/hotrod/docs/identity-keys-research/summary.xlsx
+++ b/hotrod/docs/identity-keys-research/summary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,222 +20,222 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="72">
-  <si>
-    <t>Column auto-generated by</t>
-  </si>
-  <si>
-    <t>Supports Identity</t>
-  </si>
-  <si>
-    <t>JDBC Retrieves Generated Identity Keys</t>
-  </si>
-  <si>
-    <t>Sequence Strategy</t>
-  </si>
-  <si>
-    <t>Identity Strategy</t>
-  </si>
-  <si>
-    <t>Default Strategy</t>
-  </si>
-  <si>
-    <t>Combined Retrieval</t>
-  </si>
-  <si>
-    <t>Sequence</t>
-  </si>
-  <si>
-    <t>Identity Always</t>
-  </si>
-  <si>
-    <t>Identity By Default</t>
-  </si>
-  <si>
-    <t>Pre Insert</t>
-  </si>
-  <si>
-    <t>Combi ned</t>
-  </si>
-  <si>
-    <t>Post Insert</t>
-  </si>
-  <si>
-    <t>Strategy</t>
-  </si>
-  <si>
-    <t>Multiple Values</t>
-  </si>
-  <si>
-    <t>SEQs</t>
-  </si>
-  <si>
-    <t>IDENTs</t>
-  </si>
-  <si>
-    <t>DEFs</t>
-  </si>
-  <si>
-    <t>SEQ post insert</t>
-  </si>
-  <si>
-    <t>Apache Derby  10.13</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>Single</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>N?</t>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t>GK, RN, RI</t>
-  </si>
-  <si>
-    <t>DB2 10.5</t>
-  </si>
-  <si>
-    <t>***</t>
-  </si>
-  <si>
-    <t>RN, RI, QS</t>
-  </si>
-  <si>
-    <t>values PREVIOUS VALUE FOR gen_seq1, PREVIOUS VALUE FOR gen_seq1</t>
-  </si>
-  <si>
-    <t>H2 1.3</t>
-  </si>
-  <si>
-    <t>Y*</t>
-  </si>
-  <si>
-    <t>Y**</t>
-  </si>
-  <si>
-    <t>values currval('gen_seq1'), currval('gen_seq2')</t>
-  </si>
-  <si>
-    <t>HyperSQL 2.2</t>
-  </si>
-  <si>
-    <t>GK, RI</t>
-  </si>
-  <si>
-    <t>MariaDB 5.5</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>**</t>
-  </si>
-  <si>
-    <t>MySQL 5.5</t>
-  </si>
-  <si>
-    <t>Oracle 10g</t>
-  </si>
-  <si>
-    <t>RN, RI</t>
-  </si>
-  <si>
-    <t>select gen_seq1.currval, gen_seq2.currval from dual</t>
-  </si>
-  <si>
-    <t>Oracle 12c</t>
-  </si>
-  <si>
-    <t>“</t>
-  </si>
-  <si>
-    <t>PostgreSQL 9.4</t>
-  </si>
-  <si>
-    <t>Multiple</t>
-  </si>
-  <si>
-    <t>RN, QR</t>
-  </si>
-  <si>
-    <t>select currval('gen_seq1'), currval('gen_seq2')</t>
-  </si>
-  <si>
-    <t>SAP ASE 16</t>
-  </si>
-  <si>
-    <t>SQL Server 2014</t>
-  </si>
-  <si>
-    <t>QO</t>
-  </si>
-  <si>
-    <t>SQLite</t>
-  </si>
-  <si>
-    <t>Teradata</t>
-  </si>
-  <si>
-    <t>Y?</t>
-  </si>
-  <si>
-    <t>* Max one value returned</t>
-  </si>
-  <si>
-    <t>** Unreliable when combined with triggers.</t>
-  </si>
-  <si>
-    <t>Grupo 1 - Integrado: [insert + identity + seq + default]</t>
-  </si>
-  <si>
-    <t>RN</t>
-  </si>
-  <si>
-    <t>DB2</t>
-  </si>
-  <si>
-    <t>Oracle</t>
-  </si>
-  <si>
-    <t>PostgreSQL</t>
-  </si>
-  <si>
-    <t>SQL Server</t>
-  </si>
-  <si>
-    <t>Grupo 2 - Semi Integrado [seq] -&gt; [insert + identity] -&gt; [default]</t>
-  </si>
-  <si>
-    <t>SAP ASE</t>
-  </si>
-  <si>
-    <t>MySQL</t>
-  </si>
-  <si>
-    <t>MariaDB</t>
-  </si>
-  <si>
-    <t>GK</t>
-  </si>
-  <si>
-    <t>HyperSQL</t>
-  </si>
-  <si>
-    <t>H2</t>
-  </si>
-  <si>
-    <t>Apache Derby</t>
-  </si>
-  <si>
-    <t>Grupo 3 - Rudimentario [seq] -&gt; [insert] -&gt; [identity] -&gt; [default]</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="72">
+  <si>
+    <t xml:space="preserve">Column auto-generated by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identity Columns per Table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JDBC Retrieves Generated Identity Keys</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sequence Strategy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identity Strategy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default Strategy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combined Retrieval</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sequence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identity Always</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identity By Default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pre Insert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combi ned</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Post Insert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strategy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiple Values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEQs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IDENTs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEFs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEQ post insert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apache Derby  10.13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GK, RN, RI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DB2 10.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RN, RI, QS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">values PREVIOUS VALUE FOR gen_seq1, PREVIOUS VALUE FOR gen_seq1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H2 1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">values currval('gen_seq1'), currval('gen_seq2')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HyperSQL 2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GK, RI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MariaDB 5.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MySQL 5.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oracle 10g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RN, RI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select gen_seq1.currval, gen_seq2.currval from dual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oracle 12c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PostgreSQL 9.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RN, QR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select currval('gen_seq1'), currval('gen_seq2')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAP ASE 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQL Server 2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQLite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teradata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Max one value returned</t>
+  </si>
+  <si>
+    <t xml:space="preserve">** Unreliable when combined with triggers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grupo 1 - Integrado: [insert + identity + seq + default]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DB2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oracle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PostgreSQL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQL Server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grupo 2 - Semi Integrado [seq] -&gt; [insert + identity] -&gt; [default]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAP ASE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MySQL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MariaDB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HyperSQL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apache Derby</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grupo 3 - Rudimentario [seq] -&gt; [insert] -&gt; [identity] -&gt; [default]</t>
   </si>
 </sst>
 </file>
@@ -243,7 +243,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -378,7 +378,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -451,23 +451,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -559,27 +547,26 @@
   <dimension ref="B1:W33"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="P1" activeCellId="0" sqref="P1"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q36" activeCellId="0" sqref="Q36"/>
+      <selection pane="bottomRight" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="15" min="10" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="22" min="18" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="63.4438775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="24" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="22" min="18" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="62.6377551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="24" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -842,7 +829,7 @@
       <c r="U6" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="W6" s="18" t="s">
+      <c r="W6" s="14" t="s">
         <v>33</v>
       </c>
     </row>
@@ -921,13 +908,13 @@
       <c r="H8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="K8" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="L8" s="19" t="s">
+      <c r="J8" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="K8" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="L8" s="18" t="s">
         <v>37</v>
       </c>
       <c r="M8" s="9" t="s">
@@ -948,7 +935,7 @@
       <c r="R8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="S8" s="19" t="s">
+      <c r="S8" s="18" t="s">
         <v>37</v>
       </c>
       <c r="T8" s="9" t="s">
@@ -977,13 +964,13 @@
       <c r="H9" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="J9" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="K9" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="L9" s="19" t="s">
+      <c r="J9" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="K9" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="L9" s="18" t="s">
         <v>37</v>
       </c>
       <c r="M9" s="9" t="s">
@@ -1004,7 +991,7 @@
       <c r="R9" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="S9" s="19" t="s">
+      <c r="S9" s="18" t="s">
         <v>37</v>
       </c>
       <c r="T9" s="9" t="s">
@@ -1027,7 +1014,7 @@
       <c r="E10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="F10" s="18" t="s">
         <v>37</v>
       </c>
       <c r="H10" s="11" t="s">
@@ -1042,10 +1029,10 @@
       <c r="L10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="M10" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="N10" s="19" t="s">
+      <c r="M10" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="N10" s="18" t="s">
         <v>37</v>
       </c>
       <c r="O10" s="9" t="s">
@@ -1063,7 +1050,7 @@
       <c r="S10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="T10" s="19" t="s">
+      <c r="T10" s="18" t="s">
         <v>37</v>
       </c>
       <c r="U10" s="9" t="s">
@@ -1210,13 +1197,13 @@
       <c r="H13" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="K13" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="L13" s="19" t="s">
+      <c r="J13" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="K13" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="L13" s="18" t="s">
         <v>37</v>
       </c>
       <c r="M13" s="9" t="s">
@@ -1237,7 +1224,7 @@
       <c r="R13" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="S13" s="19" t="s">
+      <c r="S13" s="18" t="s">
         <v>37</v>
       </c>
       <c r="T13" s="9" t="s">
@@ -1310,28 +1297,30 @@
       <c r="C15" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="20"/>
+      <c r="D15" s="11" t="s">
+        <v>22</v>
+      </c>
       <c r="E15" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="20"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="20"/>
-      <c r="N15" s="20"/>
-      <c r="O15" s="20"/>
-      <c r="P15" s="22"/>
-      <c r="Q15" s="23" t="s">
+      <c r="F15" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="20" t="s">
         <v>37</v>
       </c>
       <c r="R15" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="S15" s="19" t="s">
+      <c r="S15" s="18" t="s">
         <v>37</v>
       </c>
       <c r="T15" s="11" t="s">
@@ -1340,7 +1329,6 @@
       <c r="U15" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="V15" s="21"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="8" t="s">
@@ -1349,26 +1337,26 @@
       <c r="C16" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="20"/>
+      <c r="D16" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="E16" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="20"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
-      <c r="M16" s="20"/>
-      <c r="N16" s="20"/>
-      <c r="O16" s="20"/>
-      <c r="P16" s="22"/>
-      <c r="Q16" s="20"/>
+      <c r="F16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="19"/>
       <c r="R16" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="S16" s="19" t="s">
+      <c r="S16" s="18" t="s">
         <v>37</v>
       </c>
       <c r="T16" s="9" t="s">
@@ -1377,7 +1365,6 @@
       <c r="U16" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="V16" s="21"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J18" s="0" t="s">
@@ -1404,7 +1391,7 @@
       <c r="Q21" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="R21" s="24" t="s">
+      <c r="R21" s="21" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1457,7 +1444,7 @@
       <c r="Q28" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="R28" s="18" t="s">
+      <c r="R28" s="14" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1465,7 +1452,7 @@
       <c r="Q29" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="R29" s="24" t="s">
+      <c r="R29" s="21" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1473,7 +1460,7 @@
       <c r="Q30" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="R30" s="18" t="s">
+      <c r="R30" s="14" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>

<commit_message>
HOT-118 - Full identity & sequence implementation in MyBatis.
</commit_message>
<xml_diff>
--- a/hotrod/docs/identity-keys-research/summary.xlsx
+++ b/hotrod/docs/identity-keys-research/summary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="72">
   <si>
     <t xml:space="preserve">Column auto-generated by</t>
   </si>
@@ -214,6 +214,9 @@
     <t xml:space="preserve">Grupo 2 - Semi Integrado [seq] -&gt; [insert + identity] -&gt; [default]</t>
   </si>
   <si>
+    <t xml:space="preserve">GK</t>
+  </si>
+  <si>
     <t xml:space="preserve">SAP ASE</t>
   </si>
   <si>
@@ -221,9 +224,6 @@
   </si>
   <si>
     <t xml:space="preserve">MariaDB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GK</t>
   </si>
   <si>
     <t xml:space="preserve">HyperSQL</t>
@@ -281,7 +281,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -297,7 +297,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC00"/>
-        <bgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFD320"/>
       </patternFill>
     </fill>
     <fill>
@@ -326,8 +326,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFD320"/>
+        <bgColor rgb="FFFFCC00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFE6E6FF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99FFFF"/>
+        <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -378,7 +390,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -427,34 +439,42 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -463,7 +483,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -483,7 +511,7 @@
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFFD320"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
@@ -514,7 +542,7 @@
       <rgbColor rgb="FFE6E6FF"/>
       <rgbColor rgb="FFCCFF99"/>
       <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FF99FFFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCCCC"/>
@@ -547,26 +575,23 @@
   <dimension ref="B1:W33"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F18" activeCellId="0" sqref="F18"/>
+      <selection pane="bottomRight" activeCell="L24" activeCellId="0" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="1" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="22" min="18" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="62.6377551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="24" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="1" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="15" min="10" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="61.8265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1159,7 +1184,7 @@
       <c r="P12" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="Q12" s="13" t="s">
+      <c r="Q12" s="19" t="s">
         <v>47</v>
       </c>
       <c r="R12" s="9" t="s">
@@ -1215,7 +1240,7 @@
       <c r="O13" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="P13" s="12" t="s">
+      <c r="P13" s="20" t="s">
         <v>38</v>
       </c>
       <c r="Q13" s="13" t="s">
@@ -1274,7 +1299,7 @@
       <c r="P14" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="Q14" s="13" t="s">
+      <c r="Q14" s="19" t="s">
         <v>51</v>
       </c>
       <c r="R14" s="9" t="s">
@@ -1306,15 +1331,15 @@
       <c r="F15" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="19"/>
-      <c r="N15" s="19"/>
-      <c r="O15" s="19"/>
-      <c r="P15" s="12"/>
-      <c r="Q15" s="20" t="s">
+      <c r="H15" s="21"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="22" t="s">
         <v>37</v>
       </c>
       <c r="R15" s="11" t="s">
@@ -1343,16 +1368,16 @@
       <c r="E16" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
-      <c r="M16" s="19"/>
-      <c r="N16" s="19"/>
-      <c r="O16" s="19"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="19"/>
+      <c r="F16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="21"/>
+      <c r="O16" s="21"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="21"/>
       <c r="R16" s="9" t="s">
         <v>54</v>
       </c>
@@ -1375,12 +1400,17 @@
       <c r="J19" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="Q19" s="0" t="s">
+      <c r="Q19" s="23" t="s">
         <v>57</v>
       </c>
+      <c r="R19" s="23"/>
+      <c r="S19" s="23"/>
+      <c r="T19" s="23"/>
+      <c r="U19" s="23"/>
+      <c r="V19" s="23"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q20" s="12" t="s">
+      <c r="Q20" s="20" t="s">
         <v>58</v>
       </c>
       <c r="R20" s="0" t="s">
@@ -1388,15 +1418,15 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q21" s="12" t="s">
+      <c r="Q21" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="R21" s="21" t="s">
+      <c r="R21" s="24" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q22" s="12" t="s">
+      <c r="Q22" s="20" t="s">
         <v>58</v>
       </c>
       <c r="R22" s="0" t="s">
@@ -1404,7 +1434,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q23" s="12" t="s">
+      <c r="Q23" s="20" t="s">
         <v>51</v>
       </c>
       <c r="R23" s="0" t="s">
@@ -1412,52 +1442,75 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q24" s="0" t="s">
+      <c r="Q24" s="25" t="s">
         <v>63</v>
       </c>
+      <c r="R24" s="25"/>
+      <c r="S24" s="25"/>
+      <c r="T24" s="25"/>
+      <c r="U24" s="25"/>
+      <c r="V24" s="25"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q25" s="12" t="s">
+      <c r="P25" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q25" s="20" t="s">
         <v>58</v>
       </c>
       <c r="R25" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P26" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q26" s="12" t="s">
+      <c r="Q26" s="20" t="s">
         <v>58</v>
       </c>
       <c r="R26" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q27" s="12" t="s">
+      <c r="P27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q27" s="20" t="s">
         <v>58</v>
       </c>
       <c r="R27" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q28" s="12" t="s">
-        <v>67</v>
+      <c r="P28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q28" s="20" t="s">
+        <v>64</v>
       </c>
       <c r="R28" s="14" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q29" s="12" t="s">
+      <c r="P29" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q29" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="R29" s="21" t="s">
+      <c r="R29" s="24" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q30" s="12" t="s">
+      <c r="P30" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q30" s="20" t="s">
         <v>58</v>
       </c>
       <c r="R30" s="14" t="s">

</xml_diff>